<commit_message>
emails history data v2
</commit_message>
<xml_diff>
--- a/Code/public/Venator_Consuting_Exported_file_email_history_1_5.xlsx
+++ b/Code/public/Venator_Consuting_Exported_file_email_history_1_5.xlsx
@@ -433,10 +433,10 @@
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" t="str">
+        <v>mongodbteam@mongodb.com</v>
+      </c>
+      <c r="B2" t="str">
         <v>MongoDB</v>
-      </c>
-      <c r="B2" t="str">
-        <v>mongodbteam@mongodb.com</v>
       </c>
       <c r="C2" t="str">
         <v>Hamad, Mohamad</v>
@@ -488,70 +488,6 @@
       <c r="L2">
         <v>0</v>
       </c>
-      <c r="M2">
-        <v>0</v>
-      </c>
-      <c r="N2" t="str">
-        <v/>
-      </c>
-    </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A3" t="str">
-        <v>mongodbteam@mongodb.com</v>
-      </c>
-      <c r="B3" t="str">
-        <v>MongoDB</v>
-      </c>
-      <c r="C3" t="str">
-        <v>Hamad, Mohamad</v>
-      </c>
-      <c r="D3" t="str">
-        <v>/O=EXCHANGELABS/OU=EXCHANGE ADMINISTRATIVE GROUP (FYDIBOHF23SPDLT)/CN=RECIPIENTS/CN=86408E67B46E42EAAA72B2A786414236-MOHAMAD.HAM</v>
-      </c>
-      <c r="E3" t="str">
-        <v>Morgen: MongoDB Atlas 101 Workshop I Jetzt noch anmelden!</v>
-      </c>
-      <c r="F3" t="str">
-        <v> 	 
- &lt;https://s413370795.t.en25.com/e/er?utm_campaign=Int_WB_MongoDB%20101%20Workshop%20DACH_10_21_EMEA_Last%20Chance&amp;utm_medium=email&amp;utm_source=eloqua&amp;utm_term=Morgen%3A%20MongoDB%20Atlas%20101%20Workshop%20I%20Jetzt%20noch%20anmelden%21&amp;s=413370795&amp;lid=14397&amp;elqTrackId=CC4AA95D02F6A1B2EBEAA238C26499C7&amp;elq=ee9191007a7e4a19821ae21a2dfdda6f&amp;elqaid=14782&amp;elqat=1&gt;  	
-Datum: 20.10.2021
-Uhrzeit: 10 - 12 Uhr 
-Hallo Mohamad,
-hast Du Dich schon für unseren morgigen MongoDB Atlas 101 eWorkshop &lt;https://s413370795.t.en25.com/e/er?utm_campaign=Int_WB_MongoDB%20101%20Workshop%20DACH_10_21_EMEA_Last%20Chance&amp;utm_medium=email&amp;utm_source=eloqua&amp;utm_term=Morgen%3A%20MongoDB%20Atlas%20101%20Workshop%20I%20Jetzt%20noch%20anmelden%21&amp;s=413370795&amp;lid=14397&amp;elqTrackId=1ACDC2E9AC753A077030C74978391B1B&amp;elq=ee9191007a7e4a19821ae21a2dfdda6f&amp;elqaid=14782&amp;elqat=1&gt; angemeldet?
-Im Workshop lernst Du hands-on durch interaktive Übungen alle Grundlagen zu MongoDB Atlas kennen, unserer vollständig verwalteten Datenbank, und Du erfährst, wie mit Atlas Dein Datenmanagement - der bekanntlich komplexeste Teil der Anwendungsentwicklung - kinderleicht wird! Hier geht’s zur Anmeldung &lt;https://s413370795.t.en25.com/e/er?utm_campaign=Int_WB_MongoDB%20101%20Workshop%20DACH_10_21_EMEA_Last%20Chance&amp;utm_medium=email&amp;utm_source=eloqua&amp;utm_term=Morgen%3A%20MongoDB%20Atlas%20101%20Workshop%20I%20Jetzt%20noch%20anmelden%21&amp;s=413370795&amp;lid=14397&amp;elqTrackId=8FFBFFF5156B213D39ADA4D613E9D503&amp;elq=ee9191007a7e4a19821ae21a2dfdda6f&amp;elqaid=14782&amp;elqat=1&gt; .
-Im Workshop erwartet Dich:
-*	Das Erstellen einer Datenbank mit Atlas und die Sicherung der Daten
-*	Grundlegende MQL-CRUD-Operationen
-*	Erstellen von Indizes und Aggregationspipelines für komplexere Datenbankabfragen
-*	Visualisieren Deiner Daten mit MongoDB Charts
-*	Eine Live Q&amp;A Session und vieles mehr!
-Wenn Du schon immer wissen wolltest, wie Du Dein Datenmanagement optimieren und vereinfachen kannst und Dich auf die Entwicklung Deiner Anwendungen konzentrieren willst, ist dies die ideale Session für Dich!
-Jetzt noch anmelden! &lt;https://s413370795.t.en25.com/e/er?utm_campaign=Int_WB_MongoDB%20101%20Workshop%20DACH_10_21_EMEA_Last%20Chance&amp;utm_medium=email&amp;utm_source=eloqua&amp;utm_term=Morgen%3A%20MongoDB%20Atlas%20101%20Workshop%20I%20Jetzt%20noch%20anmelden%21&amp;s=413370795&amp;lid=14397&amp;elqTrackId=3DBE7AA626A677C19F35432371B21CF2&amp;elq=ee9191007a7e4a19821ae21a2dfdda6f&amp;elqaid=14782&amp;elqat=1&gt;  
-Wir freuen uns darauf, Dich im Workshop zu sehen!
-Dein MongoDB Team
- 	  &lt;https://twitter.com/MongoDB?utm_campaign=Int_WB_MongoDB%20101%20Workshop%20DACH_10_21_EMEA_Last%20Chance&amp;utm_medium=email&amp;utm_source=eloqua&amp;utm_term=Morgen%3A%20MongoDB%20Atlas%20101%20Workshop%20I%20Jetzt%20noch%20anmelden%21&amp;elqTrackId=e53813e18cb544909f1821028a585d22&amp;elq=ee9191007a7e4a19821ae21a2dfdda6f&amp;elqaid=14782&amp;elqat=1&amp;elqCampaignId=24156&gt; 	  &lt;https://www.instagram.com/mongodb/?utm_campaign=Int_WB_MongoDB%20101%20Workshop%20DACH_10_21_EMEA_Last%20Chance&amp;utm_medium=email&amp;utm_source=eloqua&amp;utm_term=Morgen%3A%20MongoDB%20Atlas%20101%20Workshop%20I%20Jetzt%20noch%20anmelden%21&amp;hl=en&amp;elqTrackId=a8a7d2e0591045ccad8ce7499f10a080&amp;elq=ee9191007a7e4a19821ae21a2dfdda6f&amp;elqaid=14782&amp;elqat=1&amp;elqCampaignId=24156&gt; 	  &lt;https://www.twitch.tv/mongodb?utm_campaign=Int_WB_MongoDB%20101%20Workshop%20DACH_10_21_EMEA_Last%20Chance&amp;utm_medium=email&amp;utm_source=eloqua&amp;utm_term=Morgen%3A%20MongoDB%20Atlas%20101%20Workshop%20I%20Jetzt%20noch%20anmelden%21&amp;elqTrackId=5a3eb5217aa64a5d8ec05cbc96d43d1a&amp;elq=ee9191007a7e4a19821ae21a2dfdda6f&amp;elqaid=14782&amp;elqat=1&amp;elqCampaignId=24156&gt; 	  &lt;https://www.linkedin.com/company/mongodbinc?utm_campaign=Int_WB_MongoDB%20101%20Workshop%20DACH_10_21_EMEA_Last%20Chance&amp;utm_medium=email&amp;utm_source=eloqua&amp;utm_term=Morgen%3A%20MongoDB%20Atlas%20101%20Workshop%20I%20Jetzt%20noch%20anmelden%21&amp;elqTrackId=77df70a4a0134f24a6fbd63284688ffc&amp;elq=ee9191007a7e4a19821ae21a2dfdda6f&amp;elqaid=14782&amp;elqat=1&amp;elqCampaignId=24156&gt; 	  	 
-MongoDB Inc., 2021. Alle Rechte vorbehalten.
-Solmsstraße 41, c/o Ralph Krone, 60486 Frankfurt am Main, Germany
-Wenn Sie keine weiteren Emails von MongoDB erhalten, oder Ihre Email-Präferenzen ändern möchten, klicken Sie hier. &lt;http://s413370795.t.en25.com/e/sl?s=413370795&amp;elq=ee9191007a7e4a19821ae21a2dfdda6f&gt;  	
-Um die Online-Version zu sehen, klicken Sie hier. &lt;https://s413370795.t.en25.com/e/es?s=413370795&amp;e=7100919&amp;elqTrackId=71ee2d8782a8479193a95cbc0f2f39b7&amp;elq=ee9191007a7e4a19821ae21a2dfdda6f&amp;elqaid=14782&amp;elqat=1&gt;  	
- &lt;https://s413370795.t.en25.com/e/FooterImages/FooterImage1?elq=ee9191007a7e4a19821ae21a2dfdda6f&amp;siteid=413370795&gt; 
-</v>
-      </c>
-      <c r="G3" t="str">
-        <v>19.10.2021</v>
-      </c>
-      <c r="I3" t="str">
-        <v>19.10.2021</v>
-      </c>
-      <c r="J3" t="str">
-        <v/>
-      </c>
-      <c r="K3" t="str">
-        <v/>
-      </c>
-      <c r="L3">
-        <v>0</v>
-      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>